<commit_message>
Lighting functional. R to change color.
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B4285F-CB55-4811-9385-8E38CFD74E0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC931B7-8839-4980-8394-41F3DE74E72A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,15 +1051,19 @@
       <c r="D4" s="24">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G67" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92))</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
@@ -1075,7 +1079,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1200,7 +1204,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 16, IF(K4+H4 &gt; 16, 16- H4, K4),0)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 16, IF(H10+I4 &gt; 16, 16- I4, H10),0)</f>
@@ -1902,11 +1906,15 @@
       <c r="D38" s="24">
         <v>1</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G38" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -2469,11 +2477,15 @@
       <c r="D63" s="24">
         <v>1</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>

</xml_diff>

<commit_message>
T and G to move lights.
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC931B7-8839-4980-8394-41F3DE74E72A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B086EB6-4E27-4443-842A-6E2A8E9436E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -936,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1070,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1079,7 +1082,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1165,11 +1168,15 @@
       <c r="D7" s="24">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>21</v>
@@ -1196,7 +1203,9 @@
       <c r="D8" s="24">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
@@ -1208,7 +1217,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 16, IF(H10+I4 &gt; 16, 16- I4, H10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 16, IF(I10+J4 &gt; 16, 16- J4, I10),0)</f>
@@ -1230,7 +1239,9 @@
       <c r="D9" s="24">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
@@ -3093,7 +3104,9 @@
       <c r="C91" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
@@ -3113,7 +3126,9 @@
       <c r="C92" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>

</xml_diff>

<commit_message>
Corvette is now using the Loader
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B086EB6-4E27-4443-842A-6E2A8E9436E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252C9273-4685-40E6-8DDC-75CAF525D6DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 16, IF(H10+I4 &gt; 16, 16- I4, H10),0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 16, IF(I10+J4 &gt; 16, 16- J4, I10),0)</f>
@@ -1599,11 +1599,15 @@
       <c r="D24" s="24">
         <v>2</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -3262,7 +3266,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fudging around. Updated rubric for extension submission.
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CC8C49-F7D7-40CA-B5A6-9649155502E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1E6D37-2671-4464-BCB1-1DE1D17EB7AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,7 +1958,9 @@
       <c r="D39" s="24">
         <v>3</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="F39" s="3"/>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
@@ -3274,7 +3276,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Attempted Transparency and Particle Systems
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1E6D37-2671-4464-BCB1-1DE1D17EB7AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C428EA9-01DE-4902-9ECF-933B08C46131}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -939,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 16, IF(H10+I4 &gt; 16, 16- I4, H10),0)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 16, IF(I10+J4 &gt; 16, 16- J4, I10),0)</f>
@@ -1961,10 +1961,12 @@
       <c r="E39" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G39" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -3276,7 +3278,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Project rubric milestone 3
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116916BC-B7ED-40DD-BD09-58ECB057B7C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7010C0AA-C4C5-4DD8-8C35-041379A91A4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,11 +1073,11 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 16, 16, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1230,11 +1230,11 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 16, IF(H10+I4 &gt; 16, 16- I4, H10),0)</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 16, IF(I10+J4 &gt; 16, 16- J4, I10),0)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1974,7 +1974,7 @@
         <v>3</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>102</v>
@@ -3297,7 +3297,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>